<commit_message>
replace buffer.name with buffer.id
</commit_message>
<xml_diff>
--- a/doc/user-guide/cookbook/buffer/alternate-materials.xlsx
+++ b/doc/user-guide/cookbook/buffer/alternate-materials.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple-community\doc\user-guide\cookbook\buffer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\frepple\community\doc\user-guide\cookbook\buffer\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2708D919-B601-443C-A3F5-7B9A5B062BF4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8025" tabRatio="731" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="731" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sales order" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <sheet name="parameter" sheetId="15" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">buffer!$A:$D</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">buffer!$A:$C</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">customer!$A:$A</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">item!$A:$C</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'item supplier'!$A:$E</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -124,24 +125,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>A @ MyFactory</t>
-  </si>
-  <si>
-    <t>B @ MyFactory</t>
-  </si>
-  <si>
-    <t>C-alt @ MyFactory</t>
-  </si>
-  <si>
-    <t>C @ MyFactory</t>
-  </si>
-  <si>
-    <t>D @ MyFactory</t>
-  </si>
-  <si>
-    <t>E @ MyFactory</t>
   </si>
   <si>
     <t>Supplier</t>
@@ -300,7 +283,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
@@ -349,7 +332,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="headerstyle" xfId="1"/>
+    <cellStyle name="headerstyle" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -649,20 +632,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -781,23 +764,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1048576"/>
+  <autoFilter ref="A1:G1048576" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="136.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="136.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -805,7 +788,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -813,162 +796,162 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1048576"/>
+  <autoFilter ref="A1:C1048576" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1043,20 +1026,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1048576"/>
+  <autoFilter ref="A1:C1048576" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -1069,22 +1052,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576"/>
+  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1098,140 +1081,118 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576"/>
+  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3">
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6">
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D1048576"/>
+  <autoFilter ref="A1:C1048576" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -1240,29 +1201,29 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A1048576"/>
+  <autoFilter ref="A1:A1048576" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1274,10 +1235,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>17</v>
@@ -1291,7 +1252,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>864000</v>
@@ -1308,7 +1269,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>864000</v>
@@ -1325,7 +1286,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>864000</v>
@@ -1342,7 +1303,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>6048000</v>
@@ -1359,7 +1320,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>864000</v>
@@ -1369,30 +1330,30 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1048576"/>
+  <autoFilter ref="A1:E1048576" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1409,27 +1370,27 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1444,10 +1405,10 @@
         <v>43511</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I2">
         <v>86400</v>
@@ -1455,7 +1416,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1470,43 +1431,43 @@
         <v>43480</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I3">
         <v>86400</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1048576"/>
+  <autoFilter ref="A1:J1048576" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -1524,12 +1485,12 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -1538,7 +1499,7 @@
         <v>-1</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1546,7 +1507,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1555,7 +1516,7 @@
         <v>-1</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1563,7 +1524,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -1572,21 +1533,21 @@
         <v>-1</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -1595,21 +1556,21 @@
         <v>-1</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1618,7 +1579,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1626,7 +1587,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -1635,7 +1596,7 @@
         <v>-1</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1643,7 +1604,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -1652,7 +1613,7 @@
         <v>-1</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1660,7 +1621,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -1669,21 +1630,21 @@
         <v>-1</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -1692,21 +1653,21 @@
         <v>-1</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1715,14 +1676,14 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1048576"/>
+  <autoFilter ref="A1:G1048576" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>